<commit_message>
new tag, new record
</commit_message>
<xml_diff>
--- a/processing_code/TutorialUniqueIDRecord.xlsx
+++ b/processing_code/TutorialUniqueIDRecord.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4111" uniqueCount="4110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4112" uniqueCount="4111">
   <si>
     <t>53641e3826d3401abc682d5896010539</t>
   </si>
@@ -12357,6 +12357,9 @@
   </si>
   <si>
     <t>NEON AOP Hyperspectral Data in HDF5 format with Python</t>
+  </si>
+  <si>
+    <t>Spatial Intro 00: Answer a Spatio-temporal Research Question with Data</t>
   </si>
 </sst>
 </file>
@@ -12687,7 +12690,7 @@
   <dimension ref="A1:B4001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13580,6 +13583,9 @@
       <c r="A111" t="s">
         <v>109</v>
       </c>
+      <c r="B111" t="s">
+        <v>4110</v>
+      </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">

</xml_diff>

<commit_message>
format DI17 hyp spec tutorials for Drupal
</commit_message>
<xml_diff>
--- a/processing_code/TutorialUniqueIDRecord.xlsx
+++ b/processing_code/TutorialUniqueIDRecord.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="460" windowWidth="24960" windowHeight="13720" tabRatio="500"/>
+    <workbookView xWindow="1180" yWindow="460" windowWidth="24960" windowHeight="13720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4115" uniqueCount="4114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4121" uniqueCount="4120">
   <si>
     <t>53641e3826d3401abc682d5896010539</t>
   </si>
@@ -12372,6 +12372,24 @@
   </si>
   <si>
     <t>Using Loops with the NEON API</t>
+  </si>
+  <si>
+    <t>Calculate NDVI in Python</t>
+  </si>
+  <si>
+    <t>Using SciKit for Support Vector Machine (SVM) Classification with Python</t>
+  </si>
+  <si>
+    <t>Classification of Hyperspectral Data with Principal Components Analysis (PCA) in Python</t>
+  </si>
+  <si>
+    <t>Classification of Hyperspectral Data with Ordinary Least Squares in Python</t>
+  </si>
+  <si>
+    <t>Band Stacking, RGB &amp; False Color Images, and Interactive Widgets in Python</t>
+  </si>
+  <si>
+    <t>Plot a Spectral Signature in Python</t>
   </si>
 </sst>
 </file>
@@ -12701,8 +12719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13627,30 +13645,48 @@
       <c r="A115" t="s">
         <v>113</v>
       </c>
+      <c r="B115" t="s">
+        <v>4114</v>
+      </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>114</v>
       </c>
+      <c r="B116" t="s">
+        <v>4115</v>
+      </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>115</v>
       </c>
+      <c r="B117" t="s">
+        <v>4116</v>
+      </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>116</v>
       </c>
+      <c r="B118" t="s">
+        <v>4117</v>
+      </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>117</v>
       </c>
+      <c r="B119" t="s">
+        <v>4118</v>
+      </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>118</v>
+      </c>
+      <c r="B120" t="s">
+        <v>4119</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add DI18 lidar for drupal format
</commit_message>
<xml_diff>
--- a/processing_code/TutorialUniqueIDRecord.xlsx
+++ b/processing_code/TutorialUniqueIDRecord.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="460" windowWidth="24960" windowHeight="13720" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="460" windowWidth="24960" windowHeight="13720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4121" uniqueCount="4120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4125" uniqueCount="4124">
   <si>
     <t>53641e3826d3401abc682d5896010539</t>
   </si>
@@ -12390,6 +12390,18 @@
   </si>
   <si>
     <t>Plot a Spectral Signature in Python</t>
+  </si>
+  <si>
+    <t>Calculate Vegetation Biomass from LiDAR Data in Python</t>
+  </si>
+  <si>
+    <t>Classify a Raster Using Threshold Values in Python</t>
+  </si>
+  <si>
+    <t>Create a Hillshade from a Terrain Raster in Python</t>
+  </si>
+  <si>
+    <t>Mask a Raster Using Threshold Values in Python</t>
   </si>
 </sst>
 </file>
@@ -12719,8 +12731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B121" sqref="B121"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="A124" sqref="A124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13693,20 +13705,32 @@
       <c r="A121" t="s">
         <v>119</v>
       </c>
+      <c r="B121" t="s">
+        <v>4120</v>
+      </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>120</v>
       </c>
+      <c r="B122" t="s">
+        <v>4121</v>
+      </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>121</v>
       </c>
+      <c r="B123" t="s">
+        <v>4122</v>
+      </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>122</v>
+      </c>
+      <c r="B124" t="s">
+        <v>4123</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add DI17 uncertainty lessons in Drupal format
</commit_message>
<xml_diff>
--- a/processing_code/TutorialUniqueIDRecord.xlsx
+++ b/processing_code/TutorialUniqueIDRecord.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4125" uniqueCount="4124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4128" uniqueCount="4127">
   <si>
     <t>53641e3826d3401abc682d5896010539</t>
   </si>
@@ -12402,6 +12402,15 @@
   </si>
   <si>
     <t>Mask a Raster Using Threshold Values in Python</t>
+  </si>
+  <si>
+    <t>Assessing Spectrometer Accuracy using Validation Tarps with Python</t>
+  </si>
+  <si>
+    <t>Hyperspectral Variation Uncertainty Analysis in Python</t>
+  </si>
+  <si>
+    <t>Exploring Uncertainty in LiDAR Data</t>
   </si>
 </sst>
 </file>
@@ -12731,8 +12740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="A124" sqref="A124"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="A127" sqref="A127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13737,15 +13746,24 @@
       <c r="A125" t="s">
         <v>123</v>
       </c>
+      <c r="B125" t="s">
+        <v>4124</v>
+      </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>124</v>
       </c>
+      <c r="B126" t="s">
+        <v>4125</v>
+      </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>125</v>
+      </c>
+      <c r="B127" t="s">
+        <v>4126</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>